<commit_message>
Ajout des graphiques aux pages mensuelles avec mise en page
</commit_message>
<xml_diff>
--- a/data/logs/waitingData.xlsx
+++ b/data/logs/waitingData.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
@@ -479,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AE97"/>
+  <dimension ref="A1:AG105"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -523,6 +523,8 @@
       <c r="AC1" s="6" t="n"/>
       <c r="AD1" s="6" t="n"/>
       <c r="AE1" s="6" t="n"/>
+      <c r="AF1" s="6" t="n"/>
+      <c r="AG1" s="6" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -680,6 +682,16 @@
           <t>2023-10-22</t>
         </is>
       </c>
+      <c r="AF2" s="4" t="inlineStr">
+        <is>
+          <t>2023-11-07</t>
+        </is>
+      </c>
+      <c r="AG2" s="4" t="inlineStr">
+        <is>
+          <t>2023-11-08</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -832,7 +844,7 @@
           <t>EELS</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AE3" s="0" t="inlineStr">
         <is>
           <t>EELS</t>
         </is>
@@ -989,9 +1001,19 @@
           <t>Null10000169</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr">
+      <c r="AE4" s="0" t="inlineStr">
         <is>
           <t>Null10000175</t>
+        </is>
+      </c>
+      <c r="AF4" s="0" t="inlineStr">
+        <is>
+          <t>Null10000183</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>Null10000189</t>
         </is>
       </c>
     </row>
@@ -1158,9 +1180,19 @@
           <t>Null10000170</t>
         </is>
       </c>
-      <c r="AE6" t="inlineStr">
+      <c r="AE6" s="0" t="inlineStr">
         <is>
           <t>Null10000176</t>
+        </is>
+      </c>
+      <c r="AF6" s="0" t="inlineStr">
+        <is>
+          <t>Null10000181</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>Null10000187</t>
         </is>
       </c>
     </row>
@@ -1315,7 +1347,7 @@
           <t>ereS|</t>
         </is>
       </c>
-      <c r="AE7" t="inlineStr">
+      <c r="AE7" s="0" t="inlineStr">
         <is>
           <t>ereS|</t>
         </is>
@@ -1484,9 +1516,19 @@
           <t>eret)</t>
         </is>
       </c>
-      <c r="AE9" t="inlineStr">
+      <c r="AE9" s="0" t="inlineStr">
         <is>
           <t>eret)</t>
+        </is>
+      </c>
+      <c r="AF9" s="0" t="inlineStr">
+        <is>
+          <t>4726989</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>4726989</t>
         </is>
       </c>
     </row>
@@ -2516,7 +2558,7 @@
           <t>Null10000172</t>
         </is>
       </c>
-      <c r="AE95" t="inlineStr">
+      <c r="AE95" s="0" t="inlineStr">
         <is>
           <t>asi</t>
         </is>
@@ -2528,7 +2570,7 @@
           <t>Null10000173</t>
         </is>
       </c>
-      <c r="AE96" t="inlineStr">
+      <c r="AE96" s="0" t="inlineStr">
         <is>
           <t>Null10000177</t>
         </is>
@@ -2540,44 +2582,152 @@
           <t>Null10000174</t>
         </is>
       </c>
-      <c r="AE97" t="inlineStr">
+      <c r="AE97" s="0" t="inlineStr">
         <is>
           <t>4751940</t>
         </is>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" s="5" t="inlineStr">
+        <is>
+          <t>Null10000178</t>
+        </is>
+      </c>
+      <c r="AF98" s="0" t="inlineStr">
+        <is>
+          <t>Null10000182</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="5" t="inlineStr">
+        <is>
+          <t>Spcpp10k</t>
+        </is>
+      </c>
+      <c r="AF99" s="0" t="inlineStr">
+        <is>
+          <t>9826343</t>
+        </is>
+      </c>
+      <c r="AG99" t="inlineStr">
+        <is>
+          <t>9826343</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="5" t="inlineStr">
+        <is>
+          <t>Null10000179</t>
+        </is>
+      </c>
+      <c r="AF100" s="0" t="inlineStr">
+        <is>
+          <t>asi</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5" t="inlineStr">
+        <is>
+          <t>RE|Brady</t>
+        </is>
+      </c>
+      <c r="AF101" s="0" t="inlineStr">
+        <is>
+          <t>808S42</t>
+        </is>
+      </c>
+      <c r="AG101" t="inlineStr">
+        <is>
+          <t>808S42</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5" t="inlineStr">
+        <is>
+          <t>Null10000180</t>
+        </is>
+      </c>
+      <c r="AF102" s="0" t="inlineStr">
+        <is>
+          <t>‘4751940</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5" t="inlineStr">
+        <is>
+          <t>Null10000184</t>
+        </is>
+      </c>
+      <c r="AG103" t="inlineStr">
+        <is>
+          <t>Null10000188</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="5" t="inlineStr">
+        <is>
+          <t>Null10000185</t>
+        </is>
+      </c>
+      <c r="AG104" t="inlineStr">
+        <is>
+          <t>asi</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="5" t="inlineStr">
+        <is>
+          <t>Null10000186</t>
+        </is>
+      </c>
+      <c r="AG105" t="inlineStr">
+        <is>
+          <t>4751940</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="B1:Y1"/>
+    <mergeCell ref="B1:V1"/>
     <mergeCell ref="B1:AB1"/>
-    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B1:AE1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="B1:X1"/>
     <mergeCell ref="B1:AD1"/>
-    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B1:AA1"/>
+    <mergeCell ref="B1:AG1"/>
+    <mergeCell ref="B1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B1:K1"/>
     <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B1:N1"/>
     <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B1"/>
-    <mergeCell ref="B1:AA1"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B1:T1"/>
+    <mergeCell ref="B1:Z1"/>
+    <mergeCell ref="B1:AF1"/>
     <mergeCell ref="B1:AC1"/>
-    <mergeCell ref="B1:U1"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B1:AE1"/>
-    <mergeCell ref="B1:W1"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B1:Y1"/>
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B1:T1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B1:V1"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B1:X1"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B1:Z1"/>
-    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>